<commit_message>
improve the graph a bit
</commit_message>
<xml_diff>
--- a/week2/5-Heap-Sort/benchmark/heap_sort_compare.xlsx
+++ b/week2/5-Heap-Sort/benchmark/heap_sort_compare.xlsx
@@ -111,6 +111,37 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -612,20 +643,83 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="267184400"/>
-        <c:axId val="267184960"/>
+        <c:axId val="141888768"/>
+        <c:axId val="141889312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="267184400"/>
+        <c:axId val="141888768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>n [count] </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44232502187226597"/>
+              <c:y val="0.89256926217556143"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -640,7 +734,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -659,7 +753,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267184960"/>
+        <c:crossAx val="141889312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -667,7 +761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="267184960"/>
+        <c:axId val="141889312"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -688,6 +782,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time [log(s)]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -719,7 +869,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267184400"/>
+        <c:crossAx val="141888768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1644,7 +1794,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>